<commit_message>
change processing type and forecast process type - workers to active workers
</commit_message>
<xml_diff>
--- a/application/src/test/resources/inbound_planning_v2_ok.xlsx
+++ b/application/src/test/resources/inbound_planning_v2_ok.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbautista/MELI_GIT/planning-model-me/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BA0900-B83C-FC48-BC78-067317FC8F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B481089-6E88-7D4E-96F8-F43615FD8F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,9 +632,6 @@
     <t>Reps por subproceso activos [HH] - NS: no sistémico, S: sistémico</t>
   </si>
   <si>
-    <t>Reps por subproceso presentes [HH] - NS: no sistémico, S: sistémico</t>
-  </si>
-  <si>
     <t>Reps por tipo [HH]</t>
   </si>
   <si>
@@ -1512,6 +1509,9 @@
   </si>
   <si>
     <t>Receiving S</t>
+  </si>
+  <si>
+    <t>Reps por subproceso efectivos [HH] - NS: no sistémico, S: sistémico</t>
   </si>
 </sst>
 </file>
@@ -4458,7 +4458,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -4516,7 +4516,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
       <c r="H6" s="30" t="s">
-        <v>186</v>
+        <v>479</v>
       </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
@@ -4524,7 +4524,7 @@
       <c r="L6" s="33"/>
       <c r="M6" s="34"/>
       <c r="N6" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O6" s="33"/>
       <c r="P6" s="33"/>
@@ -4532,12 +4532,12 @@
       <c r="R6" s="33"/>
       <c r="S6" s="34"/>
       <c r="T6" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U6" s="31"/>
       <c r="V6" s="31"/>
       <c r="W6" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="X6" s="31"/>
       <c r="Y6" s="31"/>
@@ -4548,81 +4548,81 @@
         <v>4</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="H7" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>479</v>
-      </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="K7" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="L7" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="M7" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="N7" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="T7" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>479</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="T7" s="16" t="s">
+      <c r="U7" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="V7" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="V7" s="16" t="s">
+      <c r="W7" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="X7" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="X7" s="16" t="s">
+      <c r="Y7" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Z7" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="Z7" s="16" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="8" spans="2:26" ht="15.75" customHeight="1">
       <c r="B8" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" s="18">
         <v>0</v>
@@ -4700,7 +4700,7 @@
     </row>
     <row r="9" spans="2:26" ht="15.75" customHeight="1">
       <c r="B9" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="18">
         <v>0</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="10" spans="2:26" ht="15.75" customHeight="1">
       <c r="B10" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="18">
         <v>0</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="11" spans="2:26" ht="15.75" customHeight="1">
       <c r="B11" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C11" s="18">
         <v>0</v>
@@ -4934,7 +4934,7 @@
     </row>
     <row r="12" spans="2:26" ht="15.75" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="18">
         <v>0</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="13" spans="2:26" ht="15.75" customHeight="1">
       <c r="B13" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="18">
         <v>0</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="14" spans="2:26" ht="15.75" customHeight="1">
       <c r="B14" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" s="18">
         <v>0</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="15" spans="2:26" ht="15.75" customHeight="1">
       <c r="B15" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C15" s="18">
         <v>0</v>
@@ -5246,7 +5246,7 @@
     </row>
     <row r="16" spans="2:26" ht="15.75" customHeight="1">
       <c r="B16" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="18">
         <v>0</v>
@@ -5324,7 +5324,7 @@
     </row>
     <row r="17" spans="2:26" ht="15.75" customHeight="1">
       <c r="B17" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C17" s="18">
         <v>0</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="18" spans="2:26" ht="15.75" customHeight="1">
       <c r="B18" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" s="18">
         <v>0</v>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="19" spans="2:26" ht="15.75" customHeight="1">
       <c r="B19" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C19" s="18">
         <v>0</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="20" spans="2:26" ht="15.75" customHeight="1">
       <c r="B20" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" s="18">
         <v>0</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="21" spans="2:26" ht="15.75" customHeight="1">
       <c r="B21" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C21" s="18">
         <v>0</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="22" spans="2:26" ht="15.75" customHeight="1">
       <c r="B22" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C22" s="18">
         <v>0</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="23" spans="2:26" ht="15.75" customHeight="1">
       <c r="B23" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="18">
         <v>0</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="24" spans="2:26" ht="15.75" customHeight="1">
       <c r="B24" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C24" s="18">
         <v>0</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="25" spans="2:26" ht="15.75" customHeight="1">
       <c r="B25" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C25" s="18">
         <v>0</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="26" spans="2:26" ht="15.75" customHeight="1">
       <c r="B26" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C26" s="18">
         <v>0</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="27" spans="2:26" ht="15.75" customHeight="1">
       <c r="B27" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C27" s="18">
         <v>0</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="28" spans="2:26" ht="15.75" customHeight="1">
       <c r="B28" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" s="18">
         <v>0</v>
@@ -6260,7 +6260,7 @@
     </row>
     <row r="29" spans="2:26" ht="15.75" customHeight="1">
       <c r="B29" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C29" s="18">
         <v>0</v>
@@ -6338,7 +6338,7 @@
     </row>
     <row r="30" spans="2:26" ht="15.75" customHeight="1">
       <c r="B30" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C30" s="18">
         <v>0</v>
@@ -6416,7 +6416,7 @@
     </row>
     <row r="31" spans="2:26" ht="15.75" customHeight="1">
       <c r="B31" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" s="19">
         <v>8352</v>
@@ -6494,7 +6494,7 @@
     </row>
     <row r="32" spans="2:26" ht="15.75" customHeight="1">
       <c r="B32" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C32" s="19">
         <v>8352</v>
@@ -6572,7 +6572,7 @@
     </row>
     <row r="33" spans="2:26" ht="15.75" customHeight="1">
       <c r="B33" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C33" s="19">
         <v>8352</v>
@@ -6650,7 +6650,7 @@
     </row>
     <row r="34" spans="2:26" ht="15.75" customHeight="1">
       <c r="B34" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C34" s="19">
         <v>8352</v>
@@ -6728,7 +6728,7 @@
     </row>
     <row r="35" spans="2:26" ht="15.75" customHeight="1">
       <c r="B35" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C35" s="19">
         <v>8352</v>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="36" spans="2:26" ht="15.75" customHeight="1">
       <c r="B36" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C36" s="19">
         <v>8352</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="37" spans="2:26" ht="15.75" customHeight="1">
       <c r="B37" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C37" s="19">
         <v>12528</v>
@@ -6962,7 +6962,7 @@
     </row>
     <row r="38" spans="2:26" ht="15.75" customHeight="1">
       <c r="B38" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C38" s="19">
         <v>12528</v>
@@ -7040,7 +7040,7 @@
     </row>
     <row r="39" spans="2:26" ht="15.75" customHeight="1">
       <c r="B39" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C39" s="19">
         <v>12528</v>
@@ -7118,7 +7118,7 @@
     </row>
     <row r="40" spans="2:26" ht="15.75" customHeight="1">
       <c r="B40" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C40" s="19">
         <v>12528</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="41" spans="2:26" ht="15.75" customHeight="1">
       <c r="B41" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C41" s="19">
         <v>12528</v>
@@ -7274,7 +7274,7 @@
     </row>
     <row r="42" spans="2:26" ht="15.75" customHeight="1">
       <c r="B42" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C42" s="19">
         <v>12528</v>
@@ -7352,7 +7352,7 @@
     </row>
     <row r="43" spans="2:26" ht="15.75" customHeight="1">
       <c r="B43" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C43" s="18">
         <v>0</v>
@@ -7430,7 +7430,7 @@
     </row>
     <row r="44" spans="2:26" ht="15.75" customHeight="1">
       <c r="B44" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C44" s="18">
         <v>0</v>
@@ -7508,7 +7508,7 @@
     </row>
     <row r="45" spans="2:26" ht="15.75" customHeight="1">
       <c r="B45" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C45" s="18">
         <v>0</v>
@@ -7586,7 +7586,7 @@
     </row>
     <row r="46" spans="2:26" ht="15.75" customHeight="1">
       <c r="B46" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C46" s="18">
         <v>0</v>
@@ -7664,7 +7664,7 @@
     </row>
     <row r="47" spans="2:26" ht="15.75" customHeight="1">
       <c r="B47" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C47" s="18">
         <v>0</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="48" spans="2:26" ht="15.75" customHeight="1">
       <c r="B48" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C48" s="18">
         <v>0</v>
@@ -7820,7 +7820,7 @@
     </row>
     <row r="49" spans="2:26" ht="15.75" customHeight="1">
       <c r="B49" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C49" s="18">
         <v>0</v>
@@ -7898,7 +7898,7 @@
     </row>
     <row r="50" spans="2:26" ht="15.75" customHeight="1">
       <c r="B50" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C50" s="18">
         <v>0</v>
@@ -7976,7 +7976,7 @@
     </row>
     <row r="51" spans="2:26" ht="15.75" customHeight="1">
       <c r="B51" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C51" s="18">
         <v>0</v>
@@ -8054,7 +8054,7 @@
     </row>
     <row r="52" spans="2:26" ht="15.75" customHeight="1">
       <c r="B52" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C52" s="18">
         <v>0</v>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="53" spans="2:26" ht="15.75" customHeight="1">
       <c r="B53" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C53" s="18">
         <v>0</v>
@@ -8210,7 +8210,7 @@
     </row>
     <row r="54" spans="2:26" ht="15.75" customHeight="1">
       <c r="B54" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C54" s="18">
         <v>0</v>
@@ -8288,7 +8288,7 @@
     </row>
     <row r="55" spans="2:26" ht="15.75" customHeight="1">
       <c r="B55" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C55" s="18">
         <v>0</v>
@@ -8366,7 +8366,7 @@
     </row>
     <row r="56" spans="2:26" ht="15.75" customHeight="1">
       <c r="B56" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C56" s="18">
         <v>0</v>
@@ -8444,7 +8444,7 @@
     </row>
     <row r="57" spans="2:26" ht="15.75" customHeight="1">
       <c r="B57" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C57" s="18">
         <v>0</v>
@@ -8522,7 +8522,7 @@
     </row>
     <row r="58" spans="2:26" ht="15.75" customHeight="1">
       <c r="B58" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C58" s="18">
         <v>0</v>
@@ -8600,7 +8600,7 @@
     </row>
     <row r="59" spans="2:26" ht="15.75" customHeight="1">
       <c r="B59" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C59" s="18">
         <v>0</v>
@@ -8678,7 +8678,7 @@
     </row>
     <row r="60" spans="2:26" ht="15.75" customHeight="1">
       <c r="B60" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C60" s="18">
         <v>0</v>
@@ -8756,7 +8756,7 @@
     </row>
     <row r="61" spans="2:26" ht="15.75" customHeight="1">
       <c r="B61" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C61" s="18">
         <v>0</v>
@@ -8834,7 +8834,7 @@
     </row>
     <row r="62" spans="2:26" ht="15.75" customHeight="1">
       <c r="B62" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C62" s="18">
         <v>0</v>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="63" spans="2:26" ht="15.75" customHeight="1">
       <c r="B63" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C63" s="18">
         <v>0</v>
@@ -8990,7 +8990,7 @@
     </row>
     <row r="64" spans="2:26" ht="15.75" customHeight="1">
       <c r="B64" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C64" s="18">
         <v>0</v>
@@ -9068,7 +9068,7 @@
     </row>
     <row r="65" spans="2:26" ht="15.75" customHeight="1">
       <c r="B65" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C65" s="18">
         <v>0</v>
@@ -9146,7 +9146,7 @@
     </row>
     <row r="66" spans="2:26" ht="15.75" customHeight="1">
       <c r="B66" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C66" s="18">
         <v>0</v>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="67" spans="2:26" ht="15.75" customHeight="1">
       <c r="B67" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C67" s="18">
         <v>0</v>
@@ -9302,7 +9302,7 @@
     </row>
     <row r="68" spans="2:26" ht="15.75" customHeight="1">
       <c r="B68" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C68" s="18">
         <v>0</v>
@@ -9380,7 +9380,7 @@
     </row>
     <row r="69" spans="2:26" ht="15.75" customHeight="1">
       <c r="B69" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C69" s="18">
         <v>0</v>
@@ -9458,7 +9458,7 @@
     </row>
     <row r="70" spans="2:26" ht="15.75" customHeight="1">
       <c r="B70" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C70" s="18">
         <v>0</v>
@@ -9536,7 +9536,7 @@
     </row>
     <row r="71" spans="2:26" ht="15.75" customHeight="1">
       <c r="B71" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C71" s="18">
         <v>0</v>
@@ -9614,7 +9614,7 @@
     </row>
     <row r="72" spans="2:26" ht="15.75" customHeight="1">
       <c r="B72" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C72" s="18">
         <v>0</v>
@@ -9692,7 +9692,7 @@
     </row>
     <row r="73" spans="2:26" ht="15.75" customHeight="1">
       <c r="B73" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C73" s="18">
         <v>0</v>
@@ -9770,7 +9770,7 @@
     </row>
     <row r="74" spans="2:26" ht="15.75" customHeight="1">
       <c r="B74" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C74" s="19">
         <v>8352</v>
@@ -9848,7 +9848,7 @@
     </row>
     <row r="75" spans="2:26" ht="15.75" customHeight="1">
       <c r="B75" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C75" s="19">
         <v>8352</v>
@@ -9926,7 +9926,7 @@
     </row>
     <row r="76" spans="2:26" ht="15.75" customHeight="1">
       <c r="B76" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C76" s="19">
         <v>8352</v>
@@ -10004,7 +10004,7 @@
     </row>
     <row r="77" spans="2:26" ht="15.75" customHeight="1">
       <c r="B77" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C77" s="19">
         <v>8352</v>
@@ -10082,7 +10082,7 @@
     </row>
     <row r="78" spans="2:26" ht="15.75" customHeight="1">
       <c r="B78" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C78" s="19">
         <v>8352</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="79" spans="2:26" ht="15.75" customHeight="1">
       <c r="B79" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C79" s="19">
         <v>8352</v>
@@ -10238,7 +10238,7 @@
     </row>
     <row r="80" spans="2:26" ht="15.75" customHeight="1">
       <c r="B80" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C80" s="19">
         <v>12528</v>
@@ -10316,7 +10316,7 @@
     </row>
     <row r="81" spans="2:26" ht="15.75" customHeight="1">
       <c r="B81" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C81" s="19">
         <v>12528</v>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="82" spans="2:26" ht="15.75" customHeight="1">
       <c r="B82" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C82" s="19">
         <v>12528</v>
@@ -10472,7 +10472,7 @@
     </row>
     <row r="83" spans="2:26" ht="15.75" customHeight="1">
       <c r="B83" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C83" s="19">
         <v>12528</v>
@@ -10550,7 +10550,7 @@
     </row>
     <row r="84" spans="2:26" ht="15.75" customHeight="1">
       <c r="B84" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C84" s="19">
         <v>12528</v>
@@ -10628,7 +10628,7 @@
     </row>
     <row r="85" spans="2:26" ht="15.75" customHeight="1">
       <c r="B85" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C85" s="19">
         <v>12528</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="86" spans="2:26" ht="15.75" customHeight="1">
       <c r="B86" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C86" s="18">
         <v>0</v>
@@ -10784,7 +10784,7 @@
     </row>
     <row r="87" spans="2:26" ht="15.75" customHeight="1">
       <c r="B87" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C87" s="18">
         <v>0</v>
@@ -10862,7 +10862,7 @@
     </row>
     <row r="88" spans="2:26" ht="15.75" customHeight="1">
       <c r="B88" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C88" s="18">
         <v>0</v>
@@ -10940,7 +10940,7 @@
     </row>
     <row r="89" spans="2:26" ht="15.75" customHeight="1">
       <c r="B89" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C89" s="18">
         <v>0</v>
@@ -11018,7 +11018,7 @@
     </row>
     <row r="90" spans="2:26" ht="15.75" customHeight="1">
       <c r="B90" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C90" s="18">
         <v>0</v>
@@ -11096,7 +11096,7 @@
     </row>
     <row r="91" spans="2:26" ht="15.75" customHeight="1">
       <c r="B91" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C91" s="18">
         <v>0</v>
@@ -11174,7 +11174,7 @@
     </row>
     <row r="92" spans="2:26" ht="15.75" customHeight="1">
       <c r="B92" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C92" s="18">
         <v>0</v>
@@ -11252,7 +11252,7 @@
     </row>
     <row r="93" spans="2:26" ht="15.75" customHeight="1">
       <c r="B93" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C93" s="18">
         <v>0</v>
@@ -11330,7 +11330,7 @@
     </row>
     <row r="94" spans="2:26" ht="15.75" customHeight="1">
       <c r="B94" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C94" s="18">
         <v>0</v>
@@ -11408,7 +11408,7 @@
     </row>
     <row r="95" spans="2:26" ht="15.75" customHeight="1">
       <c r="B95" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C95" s="18">
         <v>0</v>
@@ -11486,7 +11486,7 @@
     </row>
     <row r="96" spans="2:26" ht="15.75" customHeight="1">
       <c r="B96" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C96" s="18">
         <v>0</v>
@@ -11564,7 +11564,7 @@
     </row>
     <row r="97" spans="2:26" ht="15.75" customHeight="1">
       <c r="B97" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C97" s="18">
         <v>0</v>
@@ -11642,7 +11642,7 @@
     </row>
     <row r="98" spans="2:26" ht="15.75" customHeight="1">
       <c r="B98" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C98" s="18">
         <v>0</v>
@@ -11720,7 +11720,7 @@
     </row>
     <row r="99" spans="2:26" ht="15.75" customHeight="1">
       <c r="B99" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C99" s="18">
         <v>0</v>
@@ -11798,7 +11798,7 @@
     </row>
     <row r="100" spans="2:26" ht="15.75" customHeight="1">
       <c r="B100" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C100" s="18">
         <v>0</v>
@@ -11876,7 +11876,7 @@
     </row>
     <row r="101" spans="2:26" ht="15.75" customHeight="1">
       <c r="B101" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C101" s="18">
         <v>0</v>
@@ -11954,7 +11954,7 @@
     </row>
     <row r="102" spans="2:26" ht="15.75" customHeight="1">
       <c r="B102" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C102" s="18">
         <v>0</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="103" spans="2:26" ht="15.75" customHeight="1">
       <c r="B103" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C103" s="18">
         <v>0</v>
@@ -12110,7 +12110,7 @@
     </row>
     <row r="104" spans="2:26" ht="15.75" customHeight="1">
       <c r="B104" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C104" s="18">
         <v>0</v>
@@ -12188,7 +12188,7 @@
     </row>
     <row r="105" spans="2:26" ht="15.75" customHeight="1">
       <c r="B105" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C105" s="18">
         <v>0</v>
@@ -12266,7 +12266,7 @@
     </row>
     <row r="106" spans="2:26" ht="15.75" customHeight="1">
       <c r="B106" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C106" s="18">
         <v>0</v>
@@ -12344,7 +12344,7 @@
     </row>
     <row r="107" spans="2:26" ht="15.75" customHeight="1">
       <c r="B107" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C107" s="18">
         <v>0</v>
@@ -12422,7 +12422,7 @@
     </row>
     <row r="108" spans="2:26" ht="15.75" customHeight="1">
       <c r="B108" s="21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C108" s="18">
         <v>0</v>
@@ -12500,7 +12500,7 @@
     </row>
     <row r="109" spans="2:26" ht="15.75" customHeight="1">
       <c r="B109" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C109" s="18">
         <v>0</v>
@@ -12578,7 +12578,7 @@
     </row>
     <row r="110" spans="2:26" ht="15.75" customHeight="1">
       <c r="B110" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C110" s="18">
         <v>0</v>
@@ -12656,7 +12656,7 @@
     </row>
     <row r="111" spans="2:26" ht="15.75" customHeight="1">
       <c r="B111" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C111" s="18">
         <v>0</v>
@@ -12734,7 +12734,7 @@
     </row>
     <row r="112" spans="2:26" ht="15.75" customHeight="1">
       <c r="B112" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C112" s="18">
         <v>0</v>
@@ -12812,7 +12812,7 @@
     </row>
     <row r="113" spans="2:26" ht="15.75" customHeight="1">
       <c r="B113" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C113" s="18">
         <v>0</v>
@@ -12890,7 +12890,7 @@
     </row>
     <row r="114" spans="2:26" ht="15.75" customHeight="1">
       <c r="B114" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C114" s="18">
         <v>0</v>
@@ -12968,7 +12968,7 @@
     </row>
     <row r="115" spans="2:26" ht="15.75" customHeight="1">
       <c r="B115" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C115" s="18">
         <v>0</v>
@@ -13046,7 +13046,7 @@
     </row>
     <row r="116" spans="2:26" ht="15.75" customHeight="1">
       <c r="B116" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C116" s="18">
         <v>0</v>
@@ -13124,7 +13124,7 @@
     </row>
     <row r="117" spans="2:26" ht="15.75" customHeight="1">
       <c r="B117" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C117" s="19">
         <v>8352</v>
@@ -13202,7 +13202,7 @@
     </row>
     <row r="118" spans="2:26" ht="15.75" customHeight="1">
       <c r="B118" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C118" s="19">
         <v>8352</v>
@@ -13280,7 +13280,7 @@
     </row>
     <row r="119" spans="2:26" ht="15.75" customHeight="1">
       <c r="B119" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C119" s="19">
         <v>8352</v>
@@ -13358,7 +13358,7 @@
     </row>
     <row r="120" spans="2:26" ht="15.75" customHeight="1">
       <c r="B120" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C120" s="19">
         <v>8352</v>
@@ -13436,7 +13436,7 @@
     </row>
     <row r="121" spans="2:26" ht="15.75" customHeight="1">
       <c r="B121" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C121" s="19">
         <v>8352</v>
@@ -13514,7 +13514,7 @@
     </row>
     <row r="122" spans="2:26" ht="15.75" customHeight="1">
       <c r="B122" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C122" s="19">
         <v>8352</v>
@@ -13592,7 +13592,7 @@
     </row>
     <row r="123" spans="2:26" ht="15.75" customHeight="1">
       <c r="B123" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C123" s="19">
         <v>12528</v>
@@ -13670,7 +13670,7 @@
     </row>
     <row r="124" spans="2:26" ht="15.75" customHeight="1">
       <c r="B124" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C124" s="19">
         <v>12528</v>
@@ -13748,7 +13748,7 @@
     </row>
     <row r="125" spans="2:26" ht="15.75" customHeight="1">
       <c r="B125" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C125" s="19">
         <v>12528</v>
@@ -13826,7 +13826,7 @@
     </row>
     <row r="126" spans="2:26" ht="15.75" customHeight="1">
       <c r="B126" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C126" s="19">
         <v>12528</v>
@@ -13904,7 +13904,7 @@
     </row>
     <row r="127" spans="2:26" ht="15.75" customHeight="1">
       <c r="B127" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C127" s="19">
         <v>12528</v>
@@ -13982,7 +13982,7 @@
     </row>
     <row r="128" spans="2:26" ht="15.75" customHeight="1">
       <c r="B128" s="22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C128" s="19">
         <v>12528</v>
@@ -14060,7 +14060,7 @@
     </row>
     <row r="129" spans="2:26" ht="15.75" customHeight="1">
       <c r="B129" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C129" s="18">
         <v>0</v>
@@ -14138,7 +14138,7 @@
     </row>
     <row r="130" spans="2:26" ht="15.75" customHeight="1">
       <c r="B130" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C130" s="18">
         <v>0</v>
@@ -14216,7 +14216,7 @@
     </row>
     <row r="131" spans="2:26" ht="15.75" customHeight="1">
       <c r="B131" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C131" s="18">
         <v>0</v>
@@ -14294,7 +14294,7 @@
     </row>
     <row r="132" spans="2:26" ht="15.75" customHeight="1">
       <c r="B132" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C132" s="18">
         <v>0</v>
@@ -14372,7 +14372,7 @@
     </row>
     <row r="133" spans="2:26" ht="15.75" customHeight="1">
       <c r="B133" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C133" s="18">
         <v>0</v>
@@ -14450,7 +14450,7 @@
     </row>
     <row r="134" spans="2:26" ht="15.75" customHeight="1">
       <c r="B134" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C134" s="18">
         <v>0</v>
@@ -14528,7 +14528,7 @@
     </row>
     <row r="135" spans="2:26" ht="15.75" customHeight="1">
       <c r="B135" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C135" s="18">
         <v>0</v>
@@ -14606,7 +14606,7 @@
     </row>
     <row r="136" spans="2:26" ht="15.75" customHeight="1">
       <c r="B136" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C136" s="18">
         <v>0</v>
@@ -14684,7 +14684,7 @@
     </row>
     <row r="137" spans="2:26" ht="15.75" customHeight="1">
       <c r="B137" s="22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C137" s="18">
         <v>0</v>
@@ -14762,7 +14762,7 @@
     </row>
     <row r="138" spans="2:26" ht="15.75" customHeight="1">
       <c r="B138" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C138" s="18">
         <v>0</v>
@@ -14840,7 +14840,7 @@
     </row>
     <row r="139" spans="2:26" ht="15.75" customHeight="1">
       <c r="B139" s="22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C139" s="18">
         <v>0</v>
@@ -14918,7 +14918,7 @@
     </row>
     <row r="140" spans="2:26" ht="15.75" customHeight="1">
       <c r="B140" s="22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C140" s="18">
         <v>0</v>
@@ -14996,7 +14996,7 @@
     </row>
     <row r="141" spans="2:26" ht="15.75" customHeight="1">
       <c r="B141" s="22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C141" s="18">
         <v>0</v>
@@ -15074,7 +15074,7 @@
     </row>
     <row r="142" spans="2:26" ht="15.75" customHeight="1">
       <c r="B142" s="22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C142" s="18">
         <v>0</v>
@@ -15152,7 +15152,7 @@
     </row>
     <row r="143" spans="2:26" ht="15.75" customHeight="1">
       <c r="B143" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C143" s="18">
         <v>0</v>
@@ -15230,7 +15230,7 @@
     </row>
     <row r="144" spans="2:26" ht="15.75" customHeight="1">
       <c r="B144" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C144" s="18">
         <v>0</v>
@@ -15308,7 +15308,7 @@
     </row>
     <row r="145" spans="2:26" ht="15.75" customHeight="1">
       <c r="B145" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C145" s="18">
         <v>0</v>
@@ -15386,7 +15386,7 @@
     </row>
     <row r="146" spans="2:26" ht="15.75" customHeight="1">
       <c r="B146" s="22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C146" s="18">
         <v>0</v>
@@ -15464,7 +15464,7 @@
     </row>
     <row r="147" spans="2:26" ht="15.75" customHeight="1">
       <c r="B147" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C147" s="18">
         <v>0</v>
@@ -15542,7 +15542,7 @@
     </row>
     <row r="148" spans="2:26" ht="15.75" customHeight="1">
       <c r="B148" s="22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C148" s="18">
         <v>0</v>
@@ -15620,7 +15620,7 @@
     </row>
     <row r="149" spans="2:26" ht="15.75" customHeight="1">
       <c r="B149" s="22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C149" s="18">
         <v>0</v>
@@ -15698,7 +15698,7 @@
     </row>
     <row r="150" spans="2:26" ht="15.75" customHeight="1">
       <c r="B150" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C150" s="18">
         <v>0</v>
@@ -15776,7 +15776,7 @@
     </row>
     <row r="151" spans="2:26" ht="15.75" customHeight="1">
       <c r="B151" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C151" s="18">
         <v>0</v>
@@ -15854,7 +15854,7 @@
     </row>
     <row r="152" spans="2:26" ht="15.75" customHeight="1">
       <c r="B152" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C152" s="18">
         <v>0</v>
@@ -15932,7 +15932,7 @@
     </row>
     <row r="153" spans="2:26" ht="15.75" customHeight="1">
       <c r="B153" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C153" s="18">
         <v>0</v>
@@ -16010,7 +16010,7 @@
     </row>
     <row r="154" spans="2:26" ht="15.75" customHeight="1">
       <c r="B154" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C154" s="18">
         <v>0</v>
@@ -16088,7 +16088,7 @@
     </row>
     <row r="155" spans="2:26" ht="15.75" customHeight="1">
       <c r="B155" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C155" s="18">
         <v>0</v>
@@ -16166,7 +16166,7 @@
     </row>
     <row r="156" spans="2:26" ht="15.75" customHeight="1">
       <c r="B156" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C156" s="18">
         <v>0</v>
@@ -16244,7 +16244,7 @@
     </row>
     <row r="157" spans="2:26" ht="15.75" customHeight="1">
       <c r="B157" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C157" s="18">
         <v>0</v>
@@ -16322,7 +16322,7 @@
     </row>
     <row r="158" spans="2:26" ht="15.75" customHeight="1">
       <c r="B158" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C158" s="18">
         <v>0</v>
@@ -16400,7 +16400,7 @@
     </row>
     <row r="159" spans="2:26" ht="15.75" customHeight="1">
       <c r="B159" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C159" s="18">
         <v>0</v>
@@ -16478,7 +16478,7 @@
     </row>
     <row r="160" spans="2:26" ht="15.75" customHeight="1">
       <c r="B160" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C160" s="19">
         <v>8352</v>
@@ -16556,7 +16556,7 @@
     </row>
     <row r="161" spans="2:26" ht="15.75" customHeight="1">
       <c r="B161" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C161" s="19">
         <v>8352</v>
@@ -16634,7 +16634,7 @@
     </row>
     <row r="162" spans="2:26" ht="15.75" customHeight="1">
       <c r="B162" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C162" s="19">
         <v>8352</v>
@@ -16712,7 +16712,7 @@
     </row>
     <row r="163" spans="2:26" ht="15.75" customHeight="1">
       <c r="B163" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C163" s="19">
         <v>8352</v>
@@ -16790,7 +16790,7 @@
     </row>
     <row r="164" spans="2:26" ht="15.75" customHeight="1">
       <c r="B164" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C164" s="19">
         <v>8352</v>
@@ -16868,7 +16868,7 @@
     </row>
     <row r="165" spans="2:26" ht="15.75" customHeight="1">
       <c r="B165" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C165" s="19">
         <v>8352</v>
@@ -16946,7 +16946,7 @@
     </row>
     <row r="166" spans="2:26" ht="15.75" customHeight="1">
       <c r="B166" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C166" s="19">
         <v>12528</v>
@@ -17024,7 +17024,7 @@
     </row>
     <row r="167" spans="2:26" ht="15.75" customHeight="1">
       <c r="B167" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C167" s="19">
         <v>12528</v>
@@ -17102,7 +17102,7 @@
     </row>
     <row r="168" spans="2:26" ht="15.75" customHeight="1">
       <c r="B168" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C168" s="19">
         <v>12528</v>
@@ -17180,7 +17180,7 @@
     </row>
     <row r="169" spans="2:26" ht="15.75" customHeight="1">
       <c r="B169" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C169" s="19">
         <v>12528</v>
@@ -17258,7 +17258,7 @@
     </row>
     <row r="170" spans="2:26" ht="15.75" customHeight="1">
       <c r="B170" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C170" s="19">
         <v>12528</v>
@@ -17336,7 +17336,7 @@
     </row>
     <row r="171" spans="2:26" ht="15.75" customHeight="1">
       <c r="B171" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C171" s="19">
         <v>12528</v>
@@ -17414,7 +17414,7 @@
     </row>
     <row r="172" spans="2:26" ht="15.75" customHeight="1">
       <c r="B172" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C172" s="18">
         <v>0</v>
@@ -17492,7 +17492,7 @@
     </row>
     <row r="173" spans="2:26" ht="15.75" customHeight="1">
       <c r="B173" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C173" s="18">
         <v>0</v>
@@ -17570,7 +17570,7 @@
     </row>
     <row r="174" spans="2:26" ht="15.75" customHeight="1">
       <c r="B174" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C174" s="18">
         <v>0</v>
@@ -17648,7 +17648,7 @@
     </row>
     <row r="175" spans="2:26" ht="15.75" customHeight="1">
       <c r="B175" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C175" s="18">
         <v>0</v>
@@ -17738,32 +17738,32 @@
     </row>
     <row r="180" spans="2:6" ht="15.75" customHeight="1">
       <c r="B180" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="C180" s="24" t="s">
         <v>375</v>
-      </c>
-      <c r="C180" s="24" t="s">
-        <v>376</v>
       </c>
       <c r="D180" s="24"/>
       <c r="E180" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="F180" s="24" t="s">
         <v>377</v>
-      </c>
-      <c r="F180" s="24" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="181" spans="2:6" ht="15.75" customHeight="1">
       <c r="B181" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C181" s="25" t="s">
         <v>379</v>
-      </c>
-      <c r="C181" s="25" t="s">
-        <v>380</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F181" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="182" spans="2:6" ht="15.75" customHeight="1">
@@ -19058,7 +19058,7 @@
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="26"/>
       <c r="B3" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -19086,13 +19086,13 @@
     <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="26"/>
       <c r="B4" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="D4" s="28" t="s">
         <v>384</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>385</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
@@ -19118,13 +19118,13 @@
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="26"/>
       <c r="B5" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="D5" s="29" t="s">
         <v>387</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>388</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
@@ -19150,13 +19150,13 @@
     <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="26"/>
       <c r="B6" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C6" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>387</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>388</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
@@ -19182,13 +19182,13 @@
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="26"/>
       <c r="B7" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>390</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="D7" s="29" t="s">
         <v>391</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>392</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
@@ -19214,13 +19214,13 @@
     <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" s="26"/>
       <c r="B8" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>391</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>392</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
@@ -19246,13 +19246,13 @@
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="26"/>
       <c r="B9" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="D9" s="29" t="s">
         <v>395</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>396</v>
       </c>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -19278,13 +19278,13 @@
     <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="26"/>
       <c r="B10" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>398</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>399</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
@@ -19310,13 +19310,13 @@
     <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="26"/>
       <c r="B11" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>400</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>401</v>
-      </c>
       <c r="D11" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
@@ -19342,13 +19342,13 @@
     <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="26"/>
       <c r="B12" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>402</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="D12" s="29" t="s">
         <v>403</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>404</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
@@ -19374,13 +19374,13 @@
     <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="26"/>
       <c r="B13" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>405</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="D13" s="29" t="s">
         <v>406</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>407</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
@@ -19406,13 +19406,13 @@
     <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>408</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="D14" s="29" t="s">
         <v>409</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>410</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
@@ -19438,10 +19438,10 @@
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="26"/>
       <c r="B15" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>411</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>412</v>
       </c>
       <c r="D15" s="29">
         <v>0</v>
@@ -19470,10 +19470,10 @@
     <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="26"/>
       <c r="B16" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>413</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>414</v>
       </c>
       <c r="D16" s="29">
         <v>0</v>
@@ -19502,10 +19502,10 @@
     <row r="17" spans="1:24" ht="15.75" customHeight="1">
       <c r="A17" s="26"/>
       <c r="B17" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>415</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>416</v>
       </c>
       <c r="D17" s="29">
         <v>0</v>
@@ -19534,10 +19534,10 @@
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
       <c r="A18" s="26"/>
       <c r="B18" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>417</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>418</v>
       </c>
       <c r="D18" s="29">
         <v>0</v>
@@ -19566,10 +19566,10 @@
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
       <c r="A19" s="26"/>
       <c r="B19" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>419</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>420</v>
       </c>
       <c r="D19" s="29">
         <v>0</v>
@@ -19598,10 +19598,10 @@
     <row r="20" spans="1:24" ht="15.75" customHeight="1">
       <c r="A20" s="26"/>
       <c r="B20" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>421</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>422</v>
       </c>
       <c r="D20" s="29">
         <v>0</v>
@@ -19630,10 +19630,10 @@
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
       <c r="A21" s="26"/>
       <c r="B21" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>423</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>424</v>
       </c>
       <c r="D21" s="29">
         <v>0</v>
@@ -19662,10 +19662,10 @@
     <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="26"/>
       <c r="B22" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>425</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>426</v>
       </c>
       <c r="D22" s="29">
         <v>0</v>
@@ -19694,10 +19694,10 @@
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="26"/>
       <c r="B23" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>427</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>428</v>
       </c>
       <c r="D23" s="29">
         <v>0</v>
@@ -19726,10 +19726,10 @@
     <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="26"/>
       <c r="B24" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>429</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>430</v>
       </c>
       <c r="D24" s="29">
         <v>0</v>
@@ -19758,10 +19758,10 @@
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="26"/>
       <c r="B25" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>431</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>432</v>
       </c>
       <c r="D25" s="29">
         <v>0</v>
@@ -19790,10 +19790,10 @@
     <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="26"/>
       <c r="B26" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>433</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>434</v>
       </c>
       <c r="D26" s="29">
         <v>0</v>
@@ -19822,10 +19822,10 @@
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="26"/>
       <c r="B27" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>435</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>436</v>
       </c>
       <c r="D27" s="29">
         <v>0</v>
@@ -19854,10 +19854,10 @@
     <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="26"/>
       <c r="B28" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>437</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>438</v>
       </c>
       <c r="D28" s="29">
         <v>0</v>
@@ -19886,10 +19886,10 @@
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="26"/>
       <c r="B29" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>439</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>440</v>
       </c>
       <c r="D29" s="29">
         <v>0</v>
@@ -19918,10 +19918,10 @@
     <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="26"/>
       <c r="B30" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>441</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>442</v>
       </c>
       <c r="D30" s="29">
         <v>8730</v>
@@ -19950,10 +19950,10 @@
     <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="26"/>
       <c r="B31" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D31" s="29">
         <v>8730</v>
@@ -19982,10 +19982,10 @@
     <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="26"/>
       <c r="B32" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D32" s="29">
         <v>8730</v>
@@ -20014,10 +20014,10 @@
     <row r="33" spans="1:24" ht="15.75" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>445</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>446</v>
       </c>
       <c r="D33" s="29">
         <v>8730</v>
@@ -20046,10 +20046,10 @@
     <row r="34" spans="1:24" ht="15.75" customHeight="1">
       <c r="A34" s="26"/>
       <c r="B34" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>447</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>448</v>
       </c>
       <c r="D34" s="29">
         <v>8730</v>
@@ -20078,10 +20078,10 @@
     <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="26"/>
       <c r="B35" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>449</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>450</v>
       </c>
       <c r="D35" s="29">
         <v>8730</v>
@@ -20110,10 +20110,10 @@
     <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="26"/>
       <c r="B36" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>451</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>452</v>
       </c>
       <c r="D36" s="29">
         <v>13095</v>
@@ -20142,10 +20142,10 @@
     <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="26"/>
       <c r="B37" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>453</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>454</v>
       </c>
       <c r="D37" s="29">
         <v>13095</v>
@@ -20174,10 +20174,10 @@
     <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="26"/>
       <c r="B38" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>455</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>456</v>
       </c>
       <c r="D38" s="29">
         <v>13095</v>
@@ -20206,10 +20206,10 @@
     <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="26"/>
       <c r="B39" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>457</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>458</v>
       </c>
       <c r="D39" s="29">
         <v>13095</v>
@@ -20238,10 +20238,10 @@
     <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>459</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>460</v>
       </c>
       <c r="D40" s="29">
         <v>13095</v>
@@ -20270,10 +20270,10 @@
     <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="26"/>
       <c r="B41" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>461</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>462</v>
       </c>
       <c r="D41" s="29">
         <v>13095</v>
@@ -20302,10 +20302,10 @@
     <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="26"/>
       <c r="B42" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>463</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>464</v>
       </c>
       <c r="D42" s="29">
         <v>0</v>
@@ -20334,10 +20334,10 @@
     <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="26"/>
       <c r="B43" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>465</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>466</v>
       </c>
       <c r="D43" s="29">
         <v>0</v>
@@ -20366,10 +20366,10 @@
     <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="26"/>
       <c r="B44" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>467</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>468</v>
       </c>
       <c r="D44" s="29">
         <v>0</v>
@@ -20398,10 +20398,10 @@
     <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="26"/>
       <c r="B45" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>469</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>470</v>
       </c>
       <c r="D45" s="29">
         <v>0</v>
@@ -20430,10 +20430,10 @@
     <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="26"/>
       <c r="B46" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>471</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>472</v>
       </c>
       <c r="D46" s="29">
         <v>0</v>
@@ -20462,10 +20462,10 @@
     <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="26"/>
       <c r="B47" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>473</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>474</v>
       </c>
       <c r="D47" s="29">
         <v>0</v>
@@ -20494,10 +20494,10 @@
     <row r="48" spans="1:24" ht="15.75" customHeight="1">
       <c r="A48" s="26"/>
       <c r="B48" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="C48" s="29" t="s">
         <v>475</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>476</v>
       </c>
       <c r="D48" s="29">
         <v>0</v>
@@ -20526,10 +20526,10 @@
     <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="26"/>
       <c r="B49" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="C49" s="29" t="s">
         <v>477</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>478</v>
       </c>
       <c r="D49" s="29">
         <v>0</v>

</xml_diff>